<commit_message>
Update Fantasy Premier League 2022.xlsx
</commit_message>
<xml_diff>
--- a/Seasons/Fantasy Premier League 2022.xlsx
+++ b/Seasons/Fantasy Premier League 2022.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="69">
   <si>
     <t>Team</t>
   </si>
@@ -47,25 +47,31 @@
     <t>GD</t>
   </si>
   <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>Brighton</t>
+  </si>
+  <si>
+    <t>Brentford</t>
+  </si>
+  <si>
+    <t>Everton</t>
+  </si>
+  <si>
+    <t>Manchester City</t>
+  </si>
+  <si>
     <t>Manchester Utd</t>
   </si>
   <si>
     <t>Chelsea</t>
   </si>
   <si>
-    <t>Liverpool</t>
-  </si>
-  <si>
-    <t>Brentford</t>
-  </si>
-  <si>
-    <t>Everton</t>
-  </si>
-  <si>
     <t>West Ham</t>
   </si>
   <si>
-    <t>Brighton</t>
+    <t>Aston Villa</t>
   </si>
   <si>
     <t>Leicester City</t>
@@ -77,36 +83,30 @@
     <t>Watford</t>
   </si>
   <si>
-    <t>Aston Villa</t>
+    <t>Crystal Palace</t>
+  </si>
+  <si>
+    <t>Leeds United</t>
+  </si>
+  <si>
+    <t>Wolves</t>
+  </si>
+  <si>
+    <t>Arsenal</t>
+  </si>
+  <si>
+    <t>Southampton</t>
   </si>
   <si>
     <t>Burnley</t>
   </si>
   <si>
-    <t>Manchester City</t>
-  </si>
-  <si>
-    <t>Wolves</t>
-  </si>
-  <si>
-    <t>Arsenal</t>
-  </si>
-  <si>
     <t>Newcastle Utd</t>
   </si>
   <si>
-    <t>Southampton</t>
-  </si>
-  <si>
-    <t>Crystal Palace</t>
-  </si>
-  <si>
     <t>Norwich City</t>
   </si>
   <si>
-    <t>Leeds United</t>
-  </si>
-  <si>
     <t>xW</t>
   </si>
   <si>
@@ -140,15 +140,15 @@
     <t>Pts/G</t>
   </si>
   <si>
+    <t>Eli</t>
+  </si>
+  <si>
+    <t>Brandon</t>
+  </si>
+  <si>
     <t>Malachi</t>
   </si>
   <si>
-    <t>Eli</t>
-  </si>
-  <si>
-    <t>Brandon</t>
-  </si>
-  <si>
     <t>Sabastian</t>
   </si>
   <si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Eli_V_Brandon</t>
+  </si>
+  <si>
+    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -704,10 +707,10 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -716,25 +719,25 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G2">
         <v>5</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -743,16 +746,16 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R2">
         <v>1</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U2">
         <v>2022</v>
@@ -761,31 +764,31 @@
         <v>40</v>
       </c>
       <c r="W2">
+        <v>9</v>
+      </c>
+      <c r="X2">
         <v>5</v>
       </c>
-      <c r="X2">
-        <v>3</v>
-      </c>
       <c r="Y2">
         <v>0</v>
       </c>
       <c r="Z2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="AB2">
-        <v>1.8</v>
+        <v>1.67</v>
       </c>
       <c r="AC2">
         <v>13</v>
       </c>
       <c r="AD2">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="AE2">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="AG2">
         <v>1</v>
@@ -808,10 +811,10 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -820,25 +823,25 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>3</v>
       </c>
       <c r="K3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -847,16 +850,16 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U3">
         <v>2022</v>
@@ -865,31 +868,31 @@
         <v>41</v>
       </c>
       <c r="W3">
+        <v>8</v>
+      </c>
+      <c r="X3">
+        <v>4</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>3</v>
+      </c>
+      <c r="AA3">
+        <v>13</v>
+      </c>
+      <c r="AB3">
+        <v>1.62</v>
+      </c>
+      <c r="AC3">
+        <v>14</v>
+      </c>
+      <c r="AD3">
+        <v>9</v>
+      </c>
+      <c r="AE3">
         <v>5</v>
-      </c>
-      <c r="X3">
-        <v>3</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>2</v>
-      </c>
-      <c r="AA3">
-        <v>9</v>
-      </c>
-      <c r="AB3">
-        <v>1.8</v>
-      </c>
-      <c r="AC3">
-        <v>6</v>
-      </c>
-      <c r="AD3">
-        <v>7</v>
-      </c>
-      <c r="AE3">
-        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:37">
@@ -897,52 +900,52 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M4">
         <v>1</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S4">
         <v>1</v>
@@ -954,31 +957,31 @@
         <v>42</v>
       </c>
       <c r="W4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="X4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z4">
         <v>3</v>
       </c>
       <c r="AA4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AB4">
-        <v>1.2</v>
+        <v>1.43</v>
       </c>
       <c r="AC4">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="AD4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AE4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:37">
@@ -986,52 +989,52 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I5">
         <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M5">
         <v>1</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -1043,31 +1046,31 @@
         <v>43</v>
       </c>
       <c r="W5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="X5">
         <v>2</v>
       </c>
       <c r="Y5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AB5">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="AC5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AD5">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="AE5">
-        <v>-5</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="6" spans="1:37">
@@ -1075,7 +1078,7 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1084,22 +1087,22 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -1146,16 +1149,16 @@
         <v>3</v>
       </c>
       <c r="G7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -1173,10 +1176,10 @@
         <v>3</v>
       </c>
       <c r="Q7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7">
         <v>1</v>
@@ -1202,13 +1205,13 @@
         <v>3</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K8" t="s">
         <v>14</v>
@@ -1291,73 +1294,73 @@
         <v>3</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L9">
         <v>1</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9">
         <v>1</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9">
         <v>2022</v>
       </c>
       <c r="V9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W9">
+        <v>8</v>
+      </c>
+      <c r="X9">
+        <v>4</v>
+      </c>
+      <c r="Y9">
+        <v>4</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>16</v>
+      </c>
+      <c r="AB9">
+        <v>2</v>
+      </c>
+      <c r="AC9">
+        <v>14</v>
+      </c>
+      <c r="AD9">
+        <v>9</v>
+      </c>
+      <c r="AE9">
         <v>5</v>
-      </c>
-      <c r="X9">
-        <v>3</v>
-      </c>
-      <c r="Y9">
-        <v>2</v>
-      </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9">
-        <v>11</v>
-      </c>
-      <c r="AB9">
-        <v>2.2</v>
-      </c>
-      <c r="AC9">
-        <v>8</v>
-      </c>
-      <c r="AD9">
-        <v>5</v>
-      </c>
-      <c r="AE9">
-        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:37">
@@ -1365,7 +1368,7 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1374,43 +1377,43 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>3</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S10">
         <v>0</v>
@@ -1422,31 +1425,31 @@
         <v>40</v>
       </c>
       <c r="W10">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="X10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA10">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AB10">
-        <v>1.4</v>
+        <v>1.22</v>
       </c>
       <c r="AC10">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="AD10">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="AE10">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:37">
@@ -1469,16 +1472,16 @@
         <v>3</v>
       </c>
       <c r="G11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -1508,34 +1511,34 @@
         <v>2022</v>
       </c>
       <c r="V11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="X11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y11">
         <v>2</v>
       </c>
       <c r="Z11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA11">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AB11">
-        <v>1</v>
+        <v>1.14</v>
       </c>
       <c r="AC11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AD11">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AE11">
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="12" spans="1:37">
@@ -1546,28 +1549,28 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -1600,28 +1603,28 @@
         <v>43</v>
       </c>
       <c r="W12">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="X12">
         <v>1</v>
       </c>
       <c r="Y12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z12">
         <v>3</v>
       </c>
       <c r="AA12">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AB12">
-        <v>0.8</v>
+        <v>0.88</v>
       </c>
       <c r="AC12">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AD12">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AE12">
         <v>-2</v>
@@ -1632,10 +1635,10 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1644,22 +1647,22 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I13">
         <v>-1</v>
       </c>
       <c r="K13" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -1668,19 +1671,19 @@
         <v>1</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13">
         <v>1</v>
       </c>
       <c r="Q13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="14" spans="1:37">
@@ -1688,55 +1691,55 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I14">
+        <v>-3</v>
+      </c>
+      <c r="K14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>2</v>
+      </c>
+      <c r="S14">
         <v>-1</v>
-      </c>
-      <c r="K14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>1</v>
-      </c>
-      <c r="Q14">
-        <v>1</v>
-      </c>
-      <c r="R14">
-        <v>1</v>
-      </c>
-      <c r="S14">
-        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:37">
@@ -1744,52 +1747,52 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I15">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="K15" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15">
         <v>1</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S15">
         <v>-1</v>
@@ -1818,34 +1821,34 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="K16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16">
         <v>1</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S16">
         <v>-1</v>
@@ -1871,37 +1874,37 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I17">
         <v>-2</v>
       </c>
       <c r="K17" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17">
         <v>1</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S17">
         <v>-1</v>
@@ -1936,31 +1939,31 @@
         <v>-2</v>
       </c>
       <c r="K18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18">
         <v>1</v>
       </c>
       <c r="P18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S18">
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -1968,7 +1971,7 @@
         <v>26</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1977,22 +1980,22 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I19">
         <v>-3</v>
       </c>
       <c r="K19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L19">
         <v>1</v>
@@ -2024,7 +2027,7 @@
         <v>27</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -2033,22 +2036,22 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H20">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I20">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="K20" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="L20">
         <v>1</v>
@@ -2080,7 +2083,7 @@
         <v>28</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -2089,46 +2092,46 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21">
+        <v>8</v>
+      </c>
+      <c r="I21">
+        <v>-8</v>
+      </c>
+      <c r="K21" t="s">
+        <v>28</v>
+      </c>
+      <c r="L21">
+        <v>2</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>2</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
         <v>5</v>
       </c>
-      <c r="I21">
+      <c r="S21">
         <v>-4</v>
-      </c>
-      <c r="K21" t="s">
-        <v>17</v>
-      </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>1</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-      <c r="R21">
-        <v>2</v>
-      </c>
-      <c r="S21">
-        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -2257,7 +2260,7 @@
         <v>2022</v>
       </c>
       <c r="M2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -2290,16 +2293,16 @@
         <v>1</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AB2">
-        <v>3</v>
+        <v>1.142857142857143</v>
       </c>
     </row>
     <row r="3" spans="1:28">
@@ -2307,7 +2310,7 @@
         <v>2022</v>
       </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -2340,16 +2343,16 @@
         <v>0</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z3">
         <v>2</v>
       </c>
       <c r="AA3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB3">
-        <v>0</v>
+        <v>0.7142857142857143</v>
       </c>
     </row>
     <row r="4" spans="1:28">
@@ -2357,31 +2360,31 @@
         <v>2022</v>
       </c>
       <c r="M4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4">
         <v>1</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U4">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="W4" t="s">
         <v>58</v>
@@ -2404,31 +2407,31 @@
         <v>2022</v>
       </c>
       <c r="M5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5">
         <v>1</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="U5">
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="6" spans="1:28">
@@ -2436,10 +2439,10 @@
         <v>2022</v>
       </c>
       <c r="M6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -2448,16 +2451,16 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U6">
         <v>-4</v>
@@ -2500,7 +2503,7 @@
         <v>2022</v>
       </c>
       <c r="M9" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -2532,7 +2535,7 @@
         <v>2022</v>
       </c>
       <c r="M10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -2564,28 +2567,28 @@
         <v>2022</v>
       </c>
       <c r="M11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="N11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11">
         <v>1</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U11">
         <v>-1</v>
@@ -2596,28 +2599,28 @@
         <v>2022</v>
       </c>
       <c r="M12" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12">
         <v>1</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U12">
         <v>-1</v>
@@ -2628,28 +2631,28 @@
         <v>2022</v>
       </c>
       <c r="M13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="N13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13">
         <v>1</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U13">
         <v>-1</v>
@@ -2781,31 +2784,31 @@
         <v>2022</v>
       </c>
       <c r="M2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O2">
         <v>1</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="T2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W2" t="s">
         <v>59</v>
@@ -2817,13 +2820,13 @@
         <v>0</v>
       </c>
       <c r="Z2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA2">
         <v>3</v>
       </c>
       <c r="AB2">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:28">
@@ -2831,7 +2834,7 @@
         <v>2022</v>
       </c>
       <c r="M3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -2849,13 +2852,13 @@
         <v>3</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W3" t="s">
         <v>60</v>
@@ -2864,16 +2867,16 @@
         <v>2</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z3">
         <v>0</v>
       </c>
       <c r="AA3">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="AB3">
-        <v>3</v>
+        <v>1.571428571428571</v>
       </c>
     </row>
     <row r="4" spans="1:28">
@@ -2881,7 +2884,7 @@
         <v>2022</v>
       </c>
       <c r="M4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -2931,7 +2934,7 @@
         <v>2022</v>
       </c>
       <c r="M5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -2952,10 +2955,10 @@
         <v>1</v>
       </c>
       <c r="T5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U5">
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="6" spans="1:28">
@@ -2963,10 +2966,10 @@
         <v>2022</v>
       </c>
       <c r="M6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -2975,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -2984,10 +2987,10 @@
         <v>1</v>
       </c>
       <c r="T6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U6">
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="8" spans="1:28">
@@ -3027,7 +3030,7 @@
         <v>2022</v>
       </c>
       <c r="M9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -3059,7 +3062,7 @@
         <v>2022</v>
       </c>
       <c r="M10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -3091,10 +3094,10 @@
         <v>2022</v>
       </c>
       <c r="M11" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="N11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -3103,19 +3106,19 @@
         <v>1</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11">
         <v>1</v>
       </c>
       <c r="S11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="12" spans="1:28">
@@ -3123,31 +3126,31 @@
         <v>2022</v>
       </c>
       <c r="M12" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12">
         <v>1</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U12">
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="13" spans="1:28">
@@ -3308,13 +3311,13 @@
         <v>2022</v>
       </c>
       <c r="M2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -3323,22 +3326,22 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="S2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T2">
         <v>0</v>
       </c>
       <c r="U2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W2" t="s">
         <v>62</v>
       </c>
       <c r="X2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y2">
         <v>0</v>
@@ -3347,10 +3350,10 @@
         <v>1</v>
       </c>
       <c r="AA2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AB2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:28">
@@ -3358,28 +3361,28 @@
         <v>2022</v>
       </c>
       <c r="M3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U3">
         <v>2</v>
@@ -3388,19 +3391,19 @@
         <v>63</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z3">
         <v>1</v>
       </c>
       <c r="AA3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AB3">
-        <v>0</v>
+        <v>1.142857142857143</v>
       </c>
     </row>
     <row r="4" spans="1:28">
@@ -3408,13 +3411,13 @@
         <v>2022</v>
       </c>
       <c r="M4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -3423,16 +3426,16 @@
         <v>1</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T4">
         <v>3</v>
       </c>
       <c r="U4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W4" t="s">
         <v>64</v>
@@ -3458,7 +3461,7 @@
         <v>2022</v>
       </c>
       <c r="M5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -3490,7 +3493,7 @@
         <v>2022</v>
       </c>
       <c r="M6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -3554,13 +3557,13 @@
         <v>2022</v>
       </c>
       <c r="M9" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -3569,16 +3572,16 @@
         <v>0</v>
       </c>
       <c r="R9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="S9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:28">
@@ -3586,28 +3589,28 @@
         <v>2022</v>
       </c>
       <c r="M10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10">
         <v>1</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U10">
         <v>1</v>
@@ -3618,7 +3621,7 @@
         <v>2022</v>
       </c>
       <c r="M11" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -3650,28 +3653,28 @@
         <v>2022</v>
       </c>
       <c r="M12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
       <c r="R12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U12">
         <v>0</v>
@@ -3682,7 +3685,7 @@
         <v>2022</v>
       </c>
       <c r="M13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -3835,13 +3838,13 @@
         <v>2022</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -3850,16 +3853,16 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="S2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T2">
         <v>1</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W2" t="s">
         <v>65</v>
@@ -3877,7 +3880,7 @@
         <v>3</v>
       </c>
       <c r="AB2">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:28">
@@ -3885,10 +3888,10 @@
         <v>2022</v>
       </c>
       <c r="M3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O3">
         <v>1</v>
@@ -3897,19 +3900,19 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3">
         <v>3</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W3" t="s">
         <v>66</v>
@@ -3926,13 +3929,16 @@
       <c r="AA3">
         <v>0</v>
       </c>
+      <c r="AB3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="4" spans="1:28">
       <c r="L4">
         <v>2022</v>
       </c>
       <c r="M4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -3950,10 +3956,10 @@
         <v>3</v>
       </c>
       <c r="S4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U4">
         <v>1</v>
@@ -3982,13 +3988,13 @@
         <v>2022</v>
       </c>
       <c r="M5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -3997,13 +4003,13 @@
         <v>1</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U5">
         <v>-1</v>
@@ -4014,10 +4020,10 @@
         <v>2022</v>
       </c>
       <c r="M6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -4026,7 +4032,7 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -4035,10 +4041,10 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="U6">
-        <v>-3</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="8" spans="1:28">
@@ -4078,13 +4084,13 @@
         <v>2022</v>
       </c>
       <c r="M9" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -4093,16 +4099,16 @@
         <v>0</v>
       </c>
       <c r="R9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="S9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T9">
         <v>1</v>
       </c>
       <c r="U9">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:28">
@@ -4110,13 +4116,13 @@
         <v>2022</v>
       </c>
       <c r="M10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10">
         <v>1</v>
@@ -4125,16 +4131,16 @@
         <v>0</v>
       </c>
       <c r="R10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:28">
@@ -4142,10 +4148,10 @@
         <v>2022</v>
       </c>
       <c r="M11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -4154,19 +4160,19 @@
         <v>1</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11">
         <v>1</v>
       </c>
       <c r="S11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="12" spans="1:28">
@@ -4174,7 +4180,7 @@
         <v>2022</v>
       </c>
       <c r="M12" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -4206,10 +4212,10 @@
         <v>2022</v>
       </c>
       <c r="M13" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="N13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -4218,7 +4224,7 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -4227,10 +4233,10 @@
         <v>1</v>
       </c>
       <c r="T13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="U13">
-        <v>-1</v>
+        <v>-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>